<commit_message>
Bug Fixes and Removed Bot Token
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>Our TimeTable</t>
   </si>
@@ -22,28 +22,19 @@
     <t>Monday</t>
   </si>
   <si>
-    <t>PDC(BCS-6C)</t>
-  </si>
-  <si>
-    <t>CS-7</t>
-  </si>
-  <si>
-    <t>08:30-09:50</t>
-  </si>
-  <si>
-    <t>CC(BCS-6A)</t>
-  </si>
-  <si>
-    <t>E&amp;M-5</t>
-  </si>
-  <si>
-    <t>14:30-15:50</t>
-  </si>
-  <si>
-    <t>OB(BCS-6A)</t>
-  </si>
-  <si>
-    <t>CS-15</t>
+    <t>PP(BCS-7B)</t>
+  </si>
+  <si>
+    <t>CS-16</t>
+  </si>
+  <si>
+    <t>13:00-14:20</t>
+  </si>
+  <si>
+    <t>IS(BCS-7A)</t>
+  </si>
+  <si>
+    <t>CS-4</t>
   </si>
   <si>
     <t>16:00-17:20</t>
@@ -52,40 +43,16 @@
     <t>Tuesday</t>
   </si>
   <si>
-    <t>SE(BCS-6F)</t>
-  </si>
-  <si>
-    <t>E&amp;M-3</t>
-  </si>
-  <si>
-    <t>AI(BCS-6B)</t>
-  </si>
-  <si>
-    <t>CS-5</t>
-  </si>
-  <si>
-    <t>11:30-12:50</t>
+    <t>DM(BCS-7B)</t>
+  </si>
+  <si>
+    <t>CE-3</t>
   </si>
   <si>
     <t>Wednesday</t>
   </si>
   <si>
     <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>AI Lab(BCS-6B)</t>
-  </si>
-  <si>
-    <t>Lab(CS-9)</t>
-  </si>
-  <si>
-    <t>08:30-11:20</t>
   </si>
 </sst>
 </file>
@@ -101,7 +68,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,18 +99,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFD966"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF99FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -157,7 +112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -175,14 +130,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,13 +424,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D19"/>
+  <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="4" width="13.7109375" customWidth="1"/>
+    <col min="2" max="4" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -523,148 +470,77 @@
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="3" t="s">
+      <c r="D7" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="5">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>